<commit_message>
Update ANN results data
</commit_message>
<xml_diff>
--- a/results/ml models/ANN results.xlsx
+++ b/results/ml models/ANN results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitaetstgallen-my.sharepoint.com/personal/ruben_ernst_student_unisg_ch/Documents/BA/commodities-pricing/results/ml models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_D852989025269358BB7206F7463E9C0EAF3B593B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_D852989025269358BB7206F7463E9C0EAF3B593B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEF32A85-592F-40AE-8D76-C41CF0AB275F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15360" windowHeight="12620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,11 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,9 +414,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -446,7 +453,7 @@
         <v>1.8545735971525298E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -463,7 +470,7 @@
         <v>1.5588700274054301E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -480,7 +487,7 @@
         <v>2.3511828065187899E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -493,11 +500,11 @@
       <c r="D5">
         <v>0.47827423015610698</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>5.8000287702216699E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -514,7 +521,7 @@
         <v>5.41176941542943E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>

</xml_diff>